<commit_message>
Excel Results of Testing
</commit_message>
<xml_diff>
--- a/Excel Files/-1.xlsx
+++ b/Excel Files/-1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="103">
   <si>
     <t>MethodID</t>
   </si>
@@ -59,192 +59,201 @@
     <t>ExcelExporting</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>exportToExcel</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
-    <t>79</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>setClassAndPackageNames</t>
+  </si>
+  <si>
+    <t>chooseName</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>getExcelDataAsMap</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Main.java</t>
+  </si>
+  <si>
+    <t>restartReading</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>RecursiveFinder</t>
   </si>
   <si>
     <t>9</t>
   </si>
   <si>
-    <t>FALSE</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>TRUE</t>
-  </si>
-  <si>
-    <t>exportToExcel</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>setClassAndPackageNames</t>
-  </si>
-  <si>
-    <t>chooseName</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Main.java</t>
-  </si>
-  <si>
-    <t>restartReading</t>
-  </si>
-  <si>
-    <t>83</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>main</t>
+    <t>readEverything</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>SmellyClass.java</t>
+  </si>
+  <si>
+    <t>SmellyClass</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>344</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>NOM</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>WMC</t>
+  </si>
+  <si>
+    <t>LOC_Method</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>CYCLO_Method</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>isGodClass</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>isLongMethod</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>LOC_Class</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>methodName</t>
+  </si>
+  <si>
+    <t>getMethod</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>getLinesOfCode</t>
+  </si>
+  <si>
+    <t>getLinesPerMethod</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>getAreLongMethods</t>
+  </si>
+  <si>
+    <t>getCyclosPerMethod</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>getisGodClass</t>
   </si>
   <si>
     <t>25</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>RecursiveFinder</t>
-  </si>
-  <si>
-    <t>readEverything</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>SmellyClass.java</t>
-  </si>
-  <si>
-    <t>SmellyClass</t>
-  </si>
-  <si>
-    <t>344</t>
-  </si>
-  <si>
-    <t>97</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>NOM</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>WMC</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>LOC_Method</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>CYCLO_Method</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>isGodClass</t>
-  </si>
-  <si>
-    <t>94</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>isLongMethod</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>LOC_Class</t>
-  </si>
-  <si>
-    <t>methodName</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>getMethod</t>
-  </si>
-  <si>
-    <t>getLinesOfCode</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>getLinesPerMethod</t>
-  </si>
-  <si>
-    <t>getAreLongMethods</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>getCyclosPerMethod</t>
-  </si>
-  <si>
-    <t>getisGodClass</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
     <t>getWmcCount</t>
   </si>
   <si>
     <t>getMethodNames</t>
   </si>
   <si>
+    <t>27</t>
+  </si>
+  <si>
     <t>src</t>
   </si>
   <si>
@@ -257,61 +266,58 @@
     <t>131</t>
   </si>
   <si>
-    <t>27</t>
+    <t>28</t>
   </si>
   <si>
     <t>isEmpty</t>
   </si>
   <si>
-    <t>28</t>
+    <t>29</t>
   </si>
   <si>
     <t>size</t>
   </si>
   <si>
-    <t>29</t>
+    <t>30</t>
   </si>
   <si>
     <t>enqueue</t>
   </si>
   <si>
-    <t>30</t>
+    <t>31</t>
   </si>
   <si>
     <t>dequeue</t>
   </si>
   <si>
-    <t>31</t>
-  </si>
-  <si>
     <t>sample</t>
   </si>
   <si>
+    <t>33</t>
+  </si>
+  <si>
     <t>iterator</t>
   </si>
   <si>
-    <t>33</t>
-  </si>
-  <si>
     <t>34</t>
   </si>
   <si>
+    <t>35</t>
+  </si>
+  <si>
     <t>randomQueueIterator</t>
   </si>
   <si>
-    <t>35</t>
+    <t>36</t>
   </si>
   <si>
     <t>hasNext</t>
   </si>
   <si>
-    <t>36</t>
+    <t>37</t>
   </si>
   <si>
     <t>next</t>
-  </si>
-  <si>
-    <t>37</t>
   </si>
   <si>
     <t>remove</t>
@@ -356,8 +362,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
@@ -365,44 +372,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="1">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="1">
+      <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="1">
+      <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="1">
+      <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="1">
+      <c r="F1" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="1">
+      <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="1">
+      <c r="H1" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="1">
+      <c r="I1" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="1">
+      <c r="J1" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="1">
+      <c r="K1" t="s" s="2">
         <v>10</v>
       </c>
     </row>
@@ -470,7 +477,7 @@
         <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="K3" t="s">
         <v>21</v>
@@ -478,7 +485,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -487,7 +494,7 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -502,7 +509,7 @@
         <v>18</v>
       </c>
       <c r="I4" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s">
         <v>11</v>
@@ -513,7 +520,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -522,7 +529,7 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
@@ -537,7 +544,7 @@
         <v>18</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J5" t="s">
         <v>20</v>
@@ -548,34 +555,34 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
         <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
       </c>
       <c r="E6" t="s">
         <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
         <v>18</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="J6" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="K6" t="s">
         <v>21</v>
@@ -583,25 +590,25 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
         <v>34</v>
       </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="G7" t="s">
         <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" t="s">
-        <v>32</v>
       </c>
       <c r="H7" t="s">
         <v>18</v>
@@ -610,7 +617,7 @@
         <v>36</v>
       </c>
       <c r="J7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K7" t="s">
         <v>21</v>
@@ -618,34 +625,34 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
         <v>37</v>
       </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" t="s">
-        <v>38</v>
-      </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H8" t="s">
         <v>18</v>
       </c>
       <c r="I8" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K8" t="s">
         <v>21</v>
@@ -653,34 +660,34 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
         <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H9" t="s">
         <v>18</v>
       </c>
       <c r="I9" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K9" t="s">
         <v>21</v>
@@ -688,72 +695,72 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
         <v>41</v>
       </c>
-      <c r="D10" t="s">
-        <v>42</v>
-      </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="H10" t="s">
         <v>18</v>
       </c>
       <c r="I10" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="J10" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="K10" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>46</v>
       </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" t="s">
-        <v>43</v>
-      </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H11" t="s">
         <v>18</v>
       </c>
       <c r="I11" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="J11" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="K11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
@@ -764,28 +771,28 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
         <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G12" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H12" t="s">
         <v>18</v>
       </c>
       <c r="I12" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="J12" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K12" t="s">
         <v>21</v>
@@ -793,34 +800,34 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G13" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H13" t="s">
         <v>18</v>
       </c>
       <c r="I13" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="J13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K13" t="s">
         <v>21</v>
@@ -828,25 +835,25 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
         <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G14" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H14" t="s">
         <v>18</v>
@@ -855,7 +862,7 @@
         <v>54</v>
       </c>
       <c r="J14" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="K14" t="s">
         <v>21</v>
@@ -863,34 +870,34 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
         <v>55</v>
       </c>
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" t="s">
         <v>56</v>
       </c>
-      <c r="E15" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" t="s">
-        <v>44</v>
-      </c>
-      <c r="H15" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" t="s">
-        <v>57</v>
-      </c>
       <c r="J15" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="K15" t="s">
         <v>21</v>
@@ -898,34 +905,34 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" t="s">
         <v>59</v>
       </c>
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="J16" t="s">
         <v>60</v>
-      </c>
-      <c r="E16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" t="s">
-        <v>44</v>
-      </c>
-      <c r="H16" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" t="s">
-        <v>61</v>
-      </c>
-      <c r="J16" t="s">
-        <v>62</v>
       </c>
       <c r="K16" t="s">
         <v>21</v>
@@ -933,66 +940,66 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" t="s">
+        <v>62</v>
+      </c>
+      <c r="J17" t="s">
         <v>63</v>
       </c>
-      <c r="E17" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" t="s">
-        <v>44</v>
-      </c>
-      <c r="H17" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" t="s">
-        <v>28</v>
-      </c>
-      <c r="J17" t="s">
-        <v>11</v>
-      </c>
       <c r="K17" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
         <v>64</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F18" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G18" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H18" t="s">
         <v>18</v>
       </c>
       <c r="I18" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="J18" t="s">
         <v>11</v>
@@ -1009,25 +1016,25 @@
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
         <v>66</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F19" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G19" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H19" t="s">
         <v>18</v>
       </c>
       <c r="I19" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="J19" t="s">
         <v>11</v>
@@ -1038,31 +1045,31 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
         <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D20" t="s">
         <v>67</v>
       </c>
       <c r="E20" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F20" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G20" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H20" t="s">
         <v>18</v>
       </c>
       <c r="I20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J20" t="s">
         <v>11</v>
@@ -1079,25 +1086,25 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
         <v>69</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F21" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G21" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H21" t="s">
         <v>18</v>
       </c>
       <c r="I21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J21" t="s">
         <v>11</v>
@@ -1108,31 +1115,31 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
         <v>70</v>
       </c>
       <c r="E22" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F22" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G22" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H22" t="s">
         <v>18</v>
       </c>
       <c r="I22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J22" t="s">
         <v>11</v>
@@ -1149,25 +1156,25 @@
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D23" t="s">
         <v>72</v>
       </c>
       <c r="E23" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F23" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G23" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H23" t="s">
         <v>18</v>
       </c>
       <c r="I23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J23" t="s">
         <v>11</v>
@@ -1184,25 +1191,25 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
         <v>73</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F24" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G24" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H24" t="s">
         <v>18</v>
       </c>
       <c r="I24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J24" t="s">
         <v>11</v>
@@ -1219,25 +1226,25 @@
         <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D25" t="s">
         <v>75</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F25" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G25" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H25" t="s">
         <v>18</v>
       </c>
       <c r="I25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J25" t="s">
         <v>11</v>
@@ -1248,31 +1255,31 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
         <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F26" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G26" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H26" t="s">
         <v>18</v>
       </c>
       <c r="I26" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="J26" t="s">
         <v>11</v>
@@ -1286,28 +1293,28 @@
         <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" t="s">
         <v>78</v>
       </c>
-      <c r="D27" t="s">
-        <v>79</v>
-      </c>
       <c r="E27" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F27" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="G27" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="H27" t="s">
         <v>18</v>
       </c>
       <c r="I27" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="J27" t="s">
         <v>11</v>
@@ -1318,22 +1325,22 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" t="s">
         <v>81</v>
-      </c>
-      <c r="B28" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" t="s">
-        <v>78</v>
       </c>
       <c r="D28" t="s">
         <v>82</v>
       </c>
       <c r="E28" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F28" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G28" t="s">
         <v>71</v>
@@ -1353,22 +1360,22 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" t="s">
         <v>83</v>
-      </c>
-      <c r="B29" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" t="s">
-        <v>84</v>
-      </c>
-      <c r="E29" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29" t="s">
-        <v>80</v>
       </c>
       <c r="G29" t="s">
         <v>71</v>
@@ -1377,7 +1384,7 @@
         <v>18</v>
       </c>
       <c r="I29" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J29" t="s">
         <v>11</v>
@@ -1388,22 +1395,22 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D30" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E30" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F30" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G30" t="s">
         <v>71</v>
@@ -1412,33 +1419,33 @@
         <v>18</v>
       </c>
       <c r="I30" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="J30" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="K30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D31" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E31" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F31" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G31" t="s">
         <v>71</v>
@@ -1447,10 +1454,10 @@
         <v>18</v>
       </c>
       <c r="I31" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="J31" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="K31" t="s">
         <v>21</v>
@@ -1458,22 +1465,22 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D32" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E32" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F32" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G32" t="s">
         <v>71</v>
@@ -1482,10 +1489,10 @@
         <v>18</v>
       </c>
       <c r="I32" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="J32" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="K32" t="s">
         <v>21</v>
@@ -1493,22 +1500,22 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D33" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E33" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F33" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G33" t="s">
         <v>71</v>
@@ -1517,33 +1524,33 @@
         <v>18</v>
       </c>
       <c r="I33" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J33" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="K33" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D34" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="E34" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F34" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G34" t="s">
         <v>71</v>
@@ -1552,7 +1559,7 @@
         <v>18</v>
       </c>
       <c r="I34" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="J34" t="s">
         <v>11</v>
@@ -1563,22 +1570,22 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B35" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D35" t="s">
-        <v>94</v>
+        <v>37</v>
       </c>
       <c r="E35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F35" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G35" t="s">
         <v>71</v>
@@ -1587,33 +1594,33 @@
         <v>18</v>
       </c>
       <c r="I35" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J35" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="K35" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D36" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E36" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F36" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G36" t="s">
         <v>71</v>
@@ -1622,33 +1629,33 @@
         <v>18</v>
       </c>
       <c r="I36" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="J36" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="K36" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D37" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E37" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F37" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G37" t="s">
         <v>71</v>
@@ -1657,33 +1664,33 @@
         <v>18</v>
       </c>
       <c r="I37" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="J37" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="K37" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C38" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D38" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E38" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F38" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G38" t="s">
         <v>71</v>
@@ -1692,12 +1699,47 @@
         <v>18</v>
       </c>
       <c r="I38" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="J38" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="K38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B39" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" t="s">
+        <v>102</v>
+      </c>
+      <c r="E39" t="s">
+        <v>51</v>
+      </c>
+      <c r="F39" t="s">
+        <v>83</v>
+      </c>
+      <c r="G39" t="s">
+        <v>71</v>
+      </c>
+      <c r="H39" t="s">
+        <v>18</v>
+      </c>
+      <c r="I39" t="s">
+        <v>15</v>
+      </c>
+      <c r="J39" t="s">
+        <v>11</v>
+      </c>
+      <c r="K39" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Testing new methods from ExcelAPI
</commit_message>
<xml_diff>
--- a/Excel Files/-1.xlsx
+++ b/Excel Files/-1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="107">
   <si>
     <t>MethodID</t>
   </si>
@@ -321,6 +321,18 @@
   </si>
   <si>
     <t>remove</t>
+  </si>
+  <si>
+    <t>137</t>
+  </si>
+  <si>
+    <t>findInMap</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>39</t>
   </si>
 </sst>
 </file>
@@ -372,7 +384,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -427,13 +439,13 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>103</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="H2" t="s">
         <v>18</v>
@@ -462,13 +474,13 @@
         <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>103</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="H3" t="s">
         <v>18</v>
@@ -497,13 +509,13 @@
         <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>103</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="H4" t="s">
         <v>18</v>
@@ -532,13 +544,13 @@
         <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>103</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="H5" t="s">
         <v>18</v>
@@ -567,19 +579,19 @@
         <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>103</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="H6" t="s">
         <v>18</v>
       </c>
       <c r="I6" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="J6" t="s">
         <v>15</v>
@@ -596,28 +608,28 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>104</v>
       </c>
       <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" t="s">
         <v>24</v>
-      </c>
-      <c r="F7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" t="s">
-        <v>25</v>
       </c>
       <c r="K7" t="s">
         <v>21</v>
@@ -634,13 +646,13 @@
         <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
         <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>105</v>
       </c>
       <c r="G8" t="s">
         <v>35</v>
@@ -649,10 +661,10 @@
         <v>18</v>
       </c>
       <c r="I8" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="J8" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K8" t="s">
         <v>21</v>
@@ -669,13 +681,13 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
         <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>105</v>
       </c>
       <c r="G9" t="s">
         <v>35</v>
@@ -684,10 +696,10 @@
         <v>18</v>
       </c>
       <c r="I9" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="J9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="K9" t="s">
         <v>21</v>
@@ -704,13 +716,13 @@
         <v>32</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>105</v>
       </c>
       <c r="G10" t="s">
         <v>35</v>
@@ -736,31 +748,31 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="F11" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="H11" t="s">
         <v>18</v>
       </c>
       <c r="I11" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="J11" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="K11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12">
@@ -774,7 +786,7 @@
         <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
         <v>45</v>
@@ -789,13 +801,13 @@
         <v>18</v>
       </c>
       <c r="I12" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="J12" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="K12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13">
@@ -809,7 +821,7 @@
         <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
         <v>45</v>
@@ -824,10 +836,10 @@
         <v>18</v>
       </c>
       <c r="I13" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="J13" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K13" t="s">
         <v>21</v>
@@ -844,7 +856,7 @@
         <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E14" t="s">
         <v>45</v>
@@ -859,10 +871,10 @@
         <v>18</v>
       </c>
       <c r="I14" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="J14" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="K14" t="s">
         <v>21</v>
@@ -879,7 +891,7 @@
         <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
         <v>45</v>
@@ -894,10 +906,10 @@
         <v>18</v>
       </c>
       <c r="I15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J15" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="K15" t="s">
         <v>21</v>
@@ -914,7 +926,7 @@
         <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E16" t="s">
         <v>45</v>
@@ -929,10 +941,10 @@
         <v>18</v>
       </c>
       <c r="I16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J16" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="K16" t="s">
         <v>21</v>
@@ -949,7 +961,7 @@
         <v>43</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
         <v>45</v>
@@ -964,10 +976,10 @@
         <v>18</v>
       </c>
       <c r="I17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="K17" t="s">
         <v>21</v>
@@ -984,7 +996,7 @@
         <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
         <v>45</v>
@@ -999,13 +1011,13 @@
         <v>18</v>
       </c>
       <c r="I18" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="J18" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="K18" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19">
@@ -1019,7 +1031,7 @@
         <v>43</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
         <v>45</v>
@@ -1034,7 +1046,7 @@
         <v>18</v>
       </c>
       <c r="I19" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="J19" t="s">
         <v>11</v>
@@ -1054,7 +1066,7 @@
         <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E20" t="s">
         <v>45</v>
@@ -1069,7 +1081,7 @@
         <v>18</v>
       </c>
       <c r="I20" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="J20" t="s">
         <v>11</v>
@@ -1089,7 +1101,7 @@
         <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E21" t="s">
         <v>45</v>
@@ -1124,7 +1136,7 @@
         <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E22" t="s">
         <v>45</v>
@@ -1159,7 +1171,7 @@
         <v>43</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E23" t="s">
         <v>45</v>
@@ -1194,7 +1206,7 @@
         <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E24" t="s">
         <v>45</v>
@@ -1229,7 +1241,7 @@
         <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E25" t="s">
         <v>45</v>
@@ -1264,7 +1276,7 @@
         <v>43</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E26" t="s">
         <v>45</v>
@@ -1299,7 +1311,7 @@
         <v>43</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E27" t="s">
         <v>45</v>
@@ -1314,7 +1326,7 @@
         <v>18</v>
       </c>
       <c r="I27" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J27" t="s">
         <v>11</v>
@@ -1328,22 +1340,22 @@
         <v>79</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="D28" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E28" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F28" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="G28" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="H28" t="s">
         <v>18</v>
@@ -1369,7 +1381,7 @@
         <v>81</v>
       </c>
       <c r="D29" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E29" t="s">
         <v>51</v>
@@ -1384,7 +1396,7 @@
         <v>18</v>
       </c>
       <c r="I29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J29" t="s">
         <v>11</v>
@@ -1404,7 +1416,7 @@
         <v>81</v>
       </c>
       <c r="D30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E30" t="s">
         <v>51</v>
@@ -1439,7 +1451,7 @@
         <v>81</v>
       </c>
       <c r="D31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E31" t="s">
         <v>51</v>
@@ -1454,13 +1466,13 @@
         <v>18</v>
       </c>
       <c r="I31" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="J31" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="K31" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32">
@@ -1474,7 +1486,7 @@
         <v>81</v>
       </c>
       <c r="D32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E32" t="s">
         <v>51</v>
@@ -1489,7 +1501,7 @@
         <v>18</v>
       </c>
       <c r="I32" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="J32" t="s">
         <v>24</v>
@@ -1509,7 +1521,7 @@
         <v>81</v>
       </c>
       <c r="D33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E33" t="s">
         <v>51</v>
@@ -1524,10 +1536,10 @@
         <v>18</v>
       </c>
       <c r="I33" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="J33" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="K33" t="s">
         <v>21</v>
@@ -1544,7 +1556,7 @@
         <v>81</v>
       </c>
       <c r="D34" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E34" t="s">
         <v>51</v>
@@ -1559,13 +1571,13 @@
         <v>18</v>
       </c>
       <c r="I34" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J34" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="K34" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35">
@@ -1579,7 +1591,7 @@
         <v>81</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
+        <v>94</v>
       </c>
       <c r="E35" t="s">
         <v>51</v>
@@ -1594,7 +1606,7 @@
         <v>18</v>
       </c>
       <c r="I35" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="J35" t="s">
         <v>11</v>
@@ -1614,7 +1626,7 @@
         <v>81</v>
       </c>
       <c r="D36" t="s">
-        <v>97</v>
+        <v>37</v>
       </c>
       <c r="E36" t="s">
         <v>51</v>
@@ -1629,13 +1641,13 @@
         <v>18</v>
       </c>
       <c r="I36" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="J36" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="K36" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37">
@@ -1649,7 +1661,7 @@
         <v>81</v>
       </c>
       <c r="D37" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E37" t="s">
         <v>51</v>
@@ -1664,13 +1676,13 @@
         <v>18</v>
       </c>
       <c r="I37" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="J37" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="K37" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38">
@@ -1684,7 +1696,7 @@
         <v>81</v>
       </c>
       <c r="D38" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E38" t="s">
         <v>51</v>
@@ -1699,13 +1711,13 @@
         <v>18</v>
       </c>
       <c r="I38" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="J38" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="K38" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39">
@@ -1719,7 +1731,7 @@
         <v>81</v>
       </c>
       <c r="D39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E39" t="s">
         <v>51</v>
@@ -1734,12 +1746,47 @@
         <v>18</v>
       </c>
       <c r="I39" t="s">
+        <v>40</v>
+      </c>
+      <c r="J39" t="s">
+        <v>25</v>
+      </c>
+      <c r="K39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" t="s">
+        <v>102</v>
+      </c>
+      <c r="E40" t="s">
+        <v>51</v>
+      </c>
+      <c r="F40" t="s">
+        <v>83</v>
+      </c>
+      <c r="G40" t="s">
+        <v>71</v>
+      </c>
+      <c r="H40" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" t="s">
         <v>15</v>
       </c>
-      <c r="J39" t="s">
-        <v>11</v>
-      </c>
-      <c r="K39" t="s">
+      <c r="J40" t="s">
+        <v>11</v>
+      </c>
+      <c r="K40" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>